<commit_message>
integrted whole login and register
</commit_message>
<xml_diff>
--- a/WBS - Book Partner Portal.xlsx
+++ b/WBS - Book Partner Portal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PYELNE\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Book-Partner-Portal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44D54FB1-A64F-4D6A-BB13-F12CFEDA290D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF0C3C37-539F-4D40-930F-5B052EE77FD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -198,7 +198,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -632,24 +632,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C4:I76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
       <selection activeCell="F75" sqref="F75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="13.9"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.7109375" style="1"/>
-    <col min="3" max="3" width="8.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="35.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="2" width="8.7265625" style="1"/>
+    <col min="3" max="3" width="8.7265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="35.81640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.26953125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.54296875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.26953125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7265625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7265625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:9" ht="31.15" customHeight="1">
+    <row r="4" spans="3:9" ht="31.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
@@ -660,7 +660,7 @@
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
     </row>
-    <row r="5" spans="3:9" ht="28.5" customHeight="1">
+    <row r="5" spans="3:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
         <v>1</v>
       </c>
@@ -683,7 +683,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="3:9">
+    <row r="6" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C6" s="3"/>
       <c r="D6" s="4" t="s">
         <v>8</v>
@@ -691,7 +691,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="3:9">
+    <row r="7" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C7" s="3">
         <v>1</v>
       </c>
@@ -710,7 +710,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="3:9">
+    <row r="8" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -719,7 +719,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="3:9">
+    <row r="9" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -728,7 +728,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="3:9">
+    <row r="10" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C10" s="3"/>
       <c r="D10" s="4" t="s">
         <v>12</v>
@@ -737,7 +737,7 @@
       <c r="F10" s="3"/>
       <c r="I10" s="10"/>
     </row>
-    <row r="11" spans="3:9">
+    <row r="11" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C11" s="3">
         <v>1</v>
       </c>
@@ -756,7 +756,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="3:9">
+    <row r="12" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C12" s="3">
         <v>2</v>
       </c>
@@ -775,7 +775,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="3:9">
+    <row r="13" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C13" s="3">
         <v>3</v>
       </c>
@@ -794,7 +794,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="3:9">
+    <row r="14" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C14" s="3">
         <v>4</v>
       </c>
@@ -813,7 +813,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="3:9">
+    <row r="15" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C15" s="3">
         <v>5</v>
       </c>
@@ -832,7 +832,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="3:9">
+    <row r="16" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C16" s="3">
         <v>6</v>
       </c>
@@ -851,7 +851,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="3:9">
+    <row r="17" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C17" s="3">
         <v>7</v>
       </c>
@@ -870,7 +870,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="3:9">
+    <row r="18" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C18" s="3">
         <v>8</v>
       </c>
@@ -889,7 +889,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="3:9">
+    <row r="19" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C19" s="3">
         <v>9</v>
       </c>
@@ -908,7 +908,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="3:9">
+    <row r="20" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C20" s="3">
         <v>10</v>
       </c>
@@ -927,7 +927,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="3:9">
+    <row r="21" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C21" s="3">
         <v>11</v>
       </c>
@@ -946,7 +946,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="3:9">
+    <row r="22" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C22" s="3">
         <v>12</v>
       </c>
@@ -965,7 +965,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="3:9">
+    <row r="23" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C23" s="3">
         <v>13</v>
       </c>
@@ -984,7 +984,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="3:9">
+    <row r="24" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C24" s="3">
         <v>14</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="3:9">
+    <row r="25" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C25" s="3">
         <v>15</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="3:9">
+    <row r="26" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C26" s="3"/>
       <c r="D26" s="6"/>
       <c r="E26" s="3"/>
@@ -1031,7 +1031,7 @@
       <c r="H26" s="5"/>
       <c r="I26" s="8"/>
     </row>
-    <row r="27" spans="3:9">
+    <row r="27" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -1040,7 +1040,7 @@
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
     </row>
-    <row r="28" spans="3:9">
+    <row r="28" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C28" s="3"/>
       <c r="D28" s="4" t="s">
         <v>35</v>
@@ -1057,7 +1057,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="3:9">
+    <row r="29" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C29" s="3">
         <v>1</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="3:9">
+    <row r="30" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C30" s="3">
         <v>2</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="3:9">
+    <row r="31" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C31" s="3">
         <v>3</v>
       </c>
@@ -1114,7 +1114,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="3:9">
+    <row r="32" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C32" s="3">
         <v>4</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="3:9">
+    <row r="33" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C33" s="3">
         <v>5</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="3:9">
+    <row r="34" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C34" s="3">
         <v>6</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="3:9">
+    <row r="35" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
@@ -1180,7 +1180,7 @@
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
     </row>
-    <row r="36" spans="3:9">
+    <row r="36" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
@@ -1188,7 +1188,7 @@
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
     </row>
-    <row r="37" spans="3:9">
+    <row r="37" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C37" s="3"/>
       <c r="D37" s="4" t="s">
         <v>44</v>
@@ -1199,7 +1199,7 @@
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
     </row>
-    <row r="38" spans="3:9">
+    <row r="38" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C38" s="3">
         <v>1</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="3:9">
+    <row r="39" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C39" s="3">
         <v>2</v>
       </c>
@@ -1237,7 +1237,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="3:9">
+    <row r="40" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C40" s="3">
         <v>3</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="3:9">
+    <row r="41" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C41" s="3">
         <v>4</v>
       </c>
@@ -1275,7 +1275,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="3:9">
+    <row r="42" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C42" s="3">
         <v>5</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="43" spans="3:9">
+    <row r="43" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C43" s="3"/>
       <c r="D43" s="6"/>
       <c r="E43" s="3"/>
@@ -1303,7 +1303,7 @@
       <c r="H43" s="5"/>
       <c r="I43" s="9"/>
     </row>
-    <row r="44" spans="3:9">
+    <row r="44" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
@@ -1312,7 +1312,7 @@
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
     </row>
-    <row r="45" spans="3:9" ht="13.15">
+    <row r="45" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C45" s="3"/>
       <c r="D45" s="4" t="s">
         <v>51</v>
@@ -1323,7 +1323,7 @@
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
     </row>
-    <row r="46" spans="3:9" ht="13.15">
+    <row r="46" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
@@ -1332,7 +1332,7 @@
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
     </row>
-    <row r="47" spans="3:9" ht="13.15">
+    <row r="47" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
@@ -1341,7 +1341,7 @@
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
     </row>
-    <row r="48" spans="3:9" ht="13.15">
+    <row r="48" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
@@ -1350,7 +1350,7 @@
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
     </row>
-    <row r="49" spans="3:9" ht="13.15">
+    <row r="49" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
@@ -1359,7 +1359,7 @@
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
     </row>
-    <row r="50" spans="3:9" ht="13.15">
+    <row r="50" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
@@ -1368,7 +1368,7 @@
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
     </row>
-    <row r="51" spans="3:9" ht="13.15">
+    <row r="51" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
@@ -1377,7 +1377,7 @@
       <c r="H51" s="3"/>
       <c r="I51" s="3"/>
     </row>
-    <row r="52" spans="3:9" ht="13.15">
+    <row r="52" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
@@ -1386,7 +1386,7 @@
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
     </row>
-    <row r="53" spans="3:9" ht="13.15">
+    <row r="53" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
@@ -1395,7 +1395,7 @@
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
     </row>
-    <row r="54" spans="3:9" ht="13.15">
+    <row r="54" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
@@ -1404,7 +1404,7 @@
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
     </row>
-    <row r="55" spans="3:9" ht="13.15">
+    <row r="55" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
@@ -1413,7 +1413,7 @@
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
     </row>
-    <row r="56" spans="3:9" ht="13.15">
+    <row r="56" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
@@ -1422,7 +1422,7 @@
       <c r="H56" s="3"/>
       <c r="I56" s="3"/>
     </row>
-    <row r="57" spans="3:9" ht="13.15">
+    <row r="57" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
       <c r="E57" s="3"/>
@@ -1431,7 +1431,7 @@
       <c r="H57" s="3"/>
       <c r="I57" s="3"/>
     </row>
-    <row r="58" spans="3:9" ht="13.15">
+    <row r="58" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
@@ -1440,7 +1440,7 @@
       <c r="H58" s="3"/>
       <c r="I58" s="3"/>
     </row>
-    <row r="59" spans="3:9" ht="13.15">
+    <row r="59" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
@@ -1449,7 +1449,7 @@
       <c r="H59" s="3"/>
       <c r="I59" s="3"/>
     </row>
-    <row r="60" spans="3:9" ht="13.15">
+    <row r="60" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
@@ -1458,7 +1458,7 @@
       <c r="H60" s="3"/>
       <c r="I60" s="3"/>
     </row>
-    <row r="61" spans="3:9" ht="13.15">
+    <row r="61" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
@@ -1467,7 +1467,7 @@
       <c r="H61" s="3"/>
       <c r="I61" s="3"/>
     </row>
-    <row r="62" spans="3:9" ht="13.15">
+    <row r="62" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
@@ -1476,7 +1476,7 @@
       <c r="H62" s="3"/>
       <c r="I62" s="3"/>
     </row>
-    <row r="63" spans="3:9" ht="13.15">
+    <row r="63" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
@@ -1485,7 +1485,7 @@
       <c r="H63" s="3"/>
       <c r="I63" s="3"/>
     </row>
-    <row r="64" spans="3:9" ht="13.15">
+    <row r="64" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
@@ -1494,7 +1494,7 @@
       <c r="H64" s="3"/>
       <c r="I64" s="3"/>
     </row>
-    <row r="65" spans="3:9" ht="13.15">
+    <row r="65" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
@@ -1503,7 +1503,7 @@
       <c r="H65" s="3"/>
       <c r="I65" s="3"/>
     </row>
-    <row r="66" spans="3:9" ht="13.15">
+    <row r="66" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
@@ -1512,7 +1512,7 @@
       <c r="H66" s="3"/>
       <c r="I66" s="3"/>
     </row>
-    <row r="67" spans="3:9" ht="13.15">
+    <row r="67" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
@@ -1521,7 +1521,7 @@
       <c r="H67" s="3"/>
       <c r="I67" s="3"/>
     </row>
-    <row r="68" spans="3:9" ht="13.15">
+    <row r="68" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
@@ -1530,7 +1530,7 @@
       <c r="H68" s="3"/>
       <c r="I68" s="3"/>
     </row>
-    <row r="69" spans="3:9" ht="13.15">
+    <row r="69" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
       <c r="E69" s="3"/>
@@ -1539,7 +1539,7 @@
       <c r="H69" s="3"/>
       <c r="I69" s="3"/>
     </row>
-    <row r="70" spans="3:9" ht="13.15">
+    <row r="70" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
@@ -1548,7 +1548,7 @@
       <c r="H70" s="3"/>
       <c r="I70" s="3"/>
     </row>
-    <row r="71" spans="3:9" ht="13.15">
+    <row r="71" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
       <c r="E71" s="3"/>
@@ -1557,7 +1557,7 @@
       <c r="H71" s="3"/>
       <c r="I71" s="3"/>
     </row>
-    <row r="72" spans="3:9" ht="13.15">
+    <row r="72" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C72" s="3"/>
       <c r="D72" s="3"/>
       <c r="E72" s="3"/>
@@ -1566,7 +1566,7 @@
       <c r="H72" s="3"/>
       <c r="I72" s="3"/>
     </row>
-    <row r="73" spans="3:9">
+    <row r="73" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
@@ -1575,7 +1575,7 @@
       <c r="H73" s="3"/>
       <c r="I73" s="3"/>
     </row>
-    <row r="74" spans="3:9">
+    <row r="74" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
       <c r="E74" s="3"/>
@@ -1584,7 +1584,7 @@
       <c r="H74" s="3"/>
       <c r="I74" s="3"/>
     </row>
-    <row r="75" spans="3:9">
+    <row r="75" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
       <c r="E75" s="3"/>
@@ -1593,7 +1593,7 @@
       <c r="H75" s="3"/>
       <c r="I75" s="3"/>
     </row>
-    <row r="76" spans="3:9">
+    <row r="76" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
       <c r="E76" s="3"/>

</xml_diff>

<commit_message>
Added Dashboard to Angular
</commit_message>
<xml_diff>
--- a/WBS - Book Partner Portal.xlsx
+++ b/WBS - Book Partner Portal.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Book-Partner-Portal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Book-Partner-Portal-Final-Sprint-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF0C3C37-539F-4D40-930F-5B052EE77FD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59BE8F2B-A952-4EA0-82A6-EA45CF9C0123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="53">
   <si>
     <t>Work Breakdown Structure</t>
   </si>
@@ -86,18 +86,12 @@
     <t>Angular Project Creation</t>
   </si>
   <si>
-    <t>HomePage</t>
-  </si>
-  <si>
     <t>Parth</t>
   </si>
   <si>
     <t>WIP</t>
   </si>
   <si>
-    <t>Release</t>
-  </si>
-  <si>
     <t>DataBase Hosted on MsSql</t>
   </si>
   <si>
@@ -192,6 +186,15 @@
   </si>
   <si>
     <t xml:space="preserve">Deployment </t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parth </t>
+  </si>
+  <si>
+    <t>Employees Api Testing</t>
   </si>
 </sst>
 </file>
@@ -630,26 +633,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C4:I76"/>
+  <dimension ref="C4:I75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="F75" sqref="F75"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.7265625" style="1"/>
-    <col min="3" max="3" width="8.7265625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="35.81640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.26953125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.54296875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.26953125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7265625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7265625" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="2" width="8.77734375" style="1"/>
+    <col min="3" max="3" width="8.77734375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="35.77734375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.21875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.21875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.77734375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.77734375" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:9" ht="31.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
@@ -683,7 +686,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:9" ht="13.05" x14ac:dyDescent="0.3">
       <c r="C6" s="3"/>
       <c r="D6" s="4" t="s">
         <v>8</v>
@@ -691,7 +694,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:9" ht="13.05" x14ac:dyDescent="0.3">
       <c r="C7" s="3">
         <v>1</v>
       </c>
@@ -710,7 +713,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:9" ht="13.05" x14ac:dyDescent="0.3">
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -719,7 +722,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:9" ht="13.05" x14ac:dyDescent="0.3">
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -728,7 +731,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:9" ht="13.05" x14ac:dyDescent="0.3">
       <c r="C10" s="3"/>
       <c r="D10" s="4" t="s">
         <v>12</v>
@@ -737,7 +740,7 @@
       <c r="F10" s="3"/>
       <c r="I10" s="10"/>
     </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:9" ht="13.05" x14ac:dyDescent="0.3">
       <c r="C11" s="3">
         <v>1</v>
       </c>
@@ -756,7 +759,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:9" ht="13.05" x14ac:dyDescent="0.3">
       <c r="C12" s="3">
         <v>2</v>
       </c>
@@ -775,55 +778,55 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:9" ht="13.05" x14ac:dyDescent="0.3">
       <c r="C13" s="3">
         <v>3</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H13" s="5">
         <v>45108</v>
       </c>
       <c r="I13" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="3:9" ht="13.05" x14ac:dyDescent="0.3">
+      <c r="C14" s="3">
+        <v>5</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C14" s="3">
-        <v>4</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>19</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="H14" s="5">
         <v>45108</v>
       </c>
-      <c r="I14" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="I14" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="3:9" ht="13.05" x14ac:dyDescent="0.3">
       <c r="C15" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="H15" s="5">
         <v>45108</v>
@@ -832,12 +835,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:9" ht="13.05" x14ac:dyDescent="0.3">
       <c r="C16" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -851,17 +854,17 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:9" ht="13.05" x14ac:dyDescent="0.3">
       <c r="C17" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="H17" s="5">
         <v>45108</v>
@@ -870,9 +873,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:9" ht="13.05" x14ac:dyDescent="0.3">
       <c r="C18" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>23</v>
@@ -880,7 +883,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="H18" s="5">
         <v>45108</v>
@@ -889,17 +892,17 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:9" ht="13.05" x14ac:dyDescent="0.3">
       <c r="C19" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H19" s="5">
         <v>45108</v>
@@ -908,17 +911,17 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:9" ht="13.05" x14ac:dyDescent="0.3">
       <c r="C20" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="H20" s="5">
         <v>45108</v>
@@ -927,9 +930,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:9" ht="13.05" x14ac:dyDescent="0.3">
       <c r="C21" s="3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>27</v>
@@ -946,9 +949,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:9" ht="13.05" x14ac:dyDescent="0.3">
       <c r="C22" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>29</v>
@@ -965,9 +968,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:9" ht="13.05" x14ac:dyDescent="0.3">
       <c r="C23" s="3">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>31</v>
@@ -975,21 +978,21 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="H23" s="5">
-        <v>45108</v>
+        <v>45109</v>
       </c>
       <c r="I23" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:9" ht="13.05" x14ac:dyDescent="0.3">
       <c r="C24" s="3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -1003,82 +1006,76 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C25" s="3">
-        <v>15</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>34</v>
-      </c>
+    <row r="25" spans="3:9" ht="13.05" x14ac:dyDescent="0.3">
+      <c r="C25" s="3"/>
+      <c r="D25" s="6"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H25" s="5">
-        <v>45109</v>
-      </c>
-      <c r="I25" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="G25" s="3"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="8"/>
+    </row>
+    <row r="26" spans="3:9" ht="13.05" x14ac:dyDescent="0.3">
       <c r="C26" s="3"/>
-      <c r="D26" s="6"/>
+      <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="8"/>
-    </row>
-    <row r="27" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+    </row>
+    <row r="27" spans="3:9" ht="13.05" x14ac:dyDescent="0.3">
       <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
+      <c r="D27" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-    </row>
-    <row r="28" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C28" s="3"/>
-      <c r="D28" s="4" t="s">
-        <v>35</v>
+      <c r="H27" s="5"/>
+      <c r="I27" s="7"/>
+    </row>
+    <row r="28" spans="3:9" ht="13.05" x14ac:dyDescent="0.3">
+      <c r="C28" s="3">
+        <v>1</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="H28" s="5">
         <v>45110</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="29" spans="3:9" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="3:9" ht="13.05" x14ac:dyDescent="0.3">
       <c r="C29" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="H29" s="5">
         <v>45110</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" spans="3:9" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="3:9" ht="13.05" x14ac:dyDescent="0.3">
       <c r="C30" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>37</v>
@@ -1086,122 +1083,132 @@
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="H30" s="5">
         <v>45110</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="31" spans="3:9" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="3:9" ht="13.05" x14ac:dyDescent="0.3">
       <c r="C31" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H31" s="5">
         <v>45110</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="32" spans="3:9" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="3:9" ht="13.05" x14ac:dyDescent="0.3">
       <c r="C32" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="H32" s="5">
         <v>45110</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="3:9" ht="13.05" x14ac:dyDescent="0.3">
       <c r="C33" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
       <c r="G33" s="3" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="H33" s="5">
         <v>45110</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C34" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="H34" s="5">
         <v>45110</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="3:9" ht="13.05" x14ac:dyDescent="0.3">
       <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
     </row>
-    <row r="36" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:9" ht="13.05" x14ac:dyDescent="0.3">
       <c r="C36" s="3"/>
+      <c r="D36" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
     </row>
-    <row r="37" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C37" s="3"/>
-      <c r="D37" s="4" t="s">
-        <v>44</v>
+    <row r="37" spans="3:9" ht="13.05" x14ac:dyDescent="0.3">
+      <c r="C37" s="3">
+        <v>1</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-    </row>
-    <row r="38" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="G37" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H37" s="5">
+        <v>45112</v>
+      </c>
+      <c r="I37" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="3:9" ht="13.05" x14ac:dyDescent="0.3">
       <c r="C38" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>45</v>
@@ -1209,103 +1216,95 @@
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H38" s="5">
         <v>45112</v>
       </c>
       <c r="I38" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="3:9" ht="13.05" x14ac:dyDescent="0.3">
+      <c r="C39" s="3">
+        <v>3</v>
+      </c>
+      <c r="D39" s="6" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="39" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C39" s="3">
-        <v>2</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>47</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="H39" s="5">
         <v>45112</v>
       </c>
       <c r="I39" s="9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="40" spans="3:9" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40" spans="3:9" ht="13.05" x14ac:dyDescent="0.3">
       <c r="C40" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="H40" s="5">
         <v>45112</v>
       </c>
       <c r="I40" s="9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="41" spans="3:9" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="3:9" ht="13.05" x14ac:dyDescent="0.3">
       <c r="C41" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H41" s="5">
         <v>45112</v>
       </c>
       <c r="I41" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="42" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C42" s="3">
-        <v>5</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>50</v>
-      </c>
+      <c r="C42" s="3"/>
+      <c r="D42" s="6"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
-      <c r="G42" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H42" s="5">
-        <v>45112</v>
-      </c>
-      <c r="I42" s="9" t="s">
-        <v>46</v>
-      </c>
+      <c r="G42" s="3"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="9"/>
     </row>
     <row r="43" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C43" s="3"/>
-      <c r="D43" s="6"/>
+      <c r="D43" s="3"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
-      <c r="H43" s="5"/>
-      <c r="I43" s="9"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
     </row>
     <row r="44" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
+      <c r="D44" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
@@ -1314,9 +1313,7 @@
     </row>
     <row r="45" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C45" s="3"/>
-      <c r="D45" s="4" t="s">
-        <v>51</v>
-      </c>
+      <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
@@ -1593,15 +1590,6 @@
       <c r="H75" s="3"/>
       <c r="I75" s="3"/>
     </row>
-    <row r="76" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C76" s="3"/>
-      <c r="D76" s="3"/>
-      <c r="E76" s="3"/>
-      <c r="F76" s="3"/>
-      <c r="G76" s="3"/>
-      <c r="H76" s="3"/>
-      <c r="I76" s="3"/>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C4:I4"/>

</xml_diff>